<commit_message>
create '1' to excel file
</commit_message>
<xml_diff>
--- a/MircosoftExcelFile.xlsx
+++ b/MircosoftExcelFile.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9303"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
     <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010"/>
@@ -11,13 +11,13 @@
     <sheet name="Лист2" sheetId="2" r:id="rId2"/>
     <sheet name="Лист3" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="122211" fullCalcOnLoad="1"/>
+  <calcPr calcId="122211"/>
 </workbook>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -50,17 +50,22 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Обычный" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleMedium9"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Тема Office">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Стандартная">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -98,7 +103,7 @@
         <a:srgbClr val="800080"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Стандартная">
       <a:majorFont>
         <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
@@ -170,7 +175,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Стандартная">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -343,36 +348,42 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
-  <sheetData/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A1">
+        <v>1</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>